<commit_message>
update dico ajoute description et feuille tache
update dico, rajoute de description et feuille par tache
</commit_message>
<xml_diff>
--- a/ressources/stockage/dictionnaire de données.xlsx
+++ b/ressources/stockage/dictionnaire de données.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DISII\Théophile DUBOIS\projet 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coucou2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090"/>
   </bookViews>
   <sheets>
-    <sheet name="TCD" sheetId="2" r:id="rId1"/>
-    <sheet name="dictionnaire de données" sheetId="1" r:id="rId2"/>
+    <sheet name="dictionnaire de données" sheetId="1" r:id="rId1"/>
+    <sheet name="TCD" sheetId="2" r:id="rId2"/>
+    <sheet name="association" sheetId="9" r:id="rId3"/>
+    <sheet name="groupe" sheetId="8" r:id="rId4"/>
+    <sheet name="concourrir" sheetId="7" r:id="rId5"/>
+    <sheet name="session" sheetId="6" r:id="rId6"/>
+    <sheet name="user" sheetId="5" r:id="rId7"/>
+    <sheet name="license" sheetId="4" r:id="rId8"/>
+    <sheet name="paiement" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="115">
   <si>
     <t>association</t>
   </si>
@@ -138,15 +145,9 @@
     <t>idGroupeA</t>
   </si>
   <si>
-    <t>Id du groupe intérieur</t>
-  </si>
-  <si>
     <t>idGroupeB</t>
   </si>
   <si>
-    <t>Id du second groupe (intérieur ou extérieur)</t>
-  </si>
-  <si>
     <t>scoreA</t>
   </si>
   <si>
@@ -226,13 +227,166 @@
   </si>
   <si>
     <t>session</t>
+  </si>
+  <si>
+    <t>Paiment</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Concourrir</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>Identifiant de l'association</t>
+  </si>
+  <si>
+    <t>Nom de l'association</t>
+  </si>
+  <si>
+    <t>Logo de l'association</t>
+  </si>
+  <si>
+    <t>Adresse e-mail de l'association</t>
+  </si>
+  <si>
+    <t>Adresse postale de l'association</t>
+  </si>
+  <si>
+    <t>Numéro de téléphone de l'association</t>
+  </si>
+  <si>
+    <t>Adresse du site web de l'association</t>
+  </si>
+  <si>
+    <t>Date de création de l'association</t>
+  </si>
+  <si>
+    <t>Numero d'immatriculation de l'association</t>
+  </si>
+  <si>
+    <t>Identifiant du groupe</t>
+  </si>
+  <si>
+    <t>Activité du groupe</t>
+  </si>
+  <si>
+    <t>Nom du groupe</t>
+  </si>
+  <si>
+    <t>Informations relatives a l'association</t>
+  </si>
+  <si>
+    <t>Informations  relatives au groupe</t>
+  </si>
+  <si>
+    <t>Image associée au groupe</t>
+  </si>
+  <si>
+    <t>Nombre de membres du groupe</t>
+  </si>
+  <si>
+    <t>Identifiant de la session de jeux</t>
+  </si>
+  <si>
+    <t>Type de groupe: interne ou externe</t>
+  </si>
+  <si>
+    <t>Identifiant de la session de jeu</t>
+  </si>
+  <si>
+    <t>Identifiant du groupe intérieur</t>
+  </si>
+  <si>
+    <t>Identifiant du second groupe (peu être intérieur ou extérieur)</t>
+  </si>
+  <si>
+    <t>Identifiant de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Pseudo de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Nom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Prénom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Numéro de téléphone de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Numéro de téléphone portable de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Adresse postale de l'uutilisateur</t>
+  </si>
+  <si>
+    <t>Adresse mail de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Date de naissance de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Type de compte: Licencié, non licencié, administrateur, gestionnaire…</t>
+  </si>
+  <si>
+    <t>Mot de passe de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Identifiant de la license utilisateur</t>
+  </si>
+  <si>
+    <t>Identifiant du groupe de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Identifiant de licence</t>
+  </si>
+  <si>
+    <t>Identifiant du paiement de la licence</t>
+  </si>
+  <si>
+    <t>Date d'acquisition de la licence</t>
+  </si>
+  <si>
+    <t>Type de licence (0, 1, 2) pour le renouvellement des licence  (e-mail)</t>
+  </si>
+  <si>
+    <t>Type de règlement (espece, CB, chéque)</t>
+  </si>
+  <si>
+    <t>Montant du paiement</t>
+  </si>
+  <si>
+    <t>Date du paiment</t>
+  </si>
+  <si>
+    <t>Identifiant de la licence</t>
+  </si>
+  <si>
+    <t>Score du groupe A relevé en fin de session</t>
+  </si>
+  <si>
+    <t>Score du groupe B relevé en fin de session</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,8 +408,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +430,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -277,11 +451,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -292,12 +556,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,7 +597,7 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -432,7 +723,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -950,7 +1241,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A59" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -1202,15 +1493,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:F50" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:F50" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:F50"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="table" dataDxfId="7"/>
-    <tableColumn id="2" name="rubrique" dataDxfId="6"/>
-    <tableColumn id="3" name="type" dataDxfId="5"/>
-    <tableColumn id="4" name="taille" dataDxfId="4"/>
-    <tableColumn id="5" name="commentaire" dataDxfId="3"/>
-    <tableColumn id="6" name="clé" dataDxfId="2"/>
+    <tableColumn id="1" name="table" dataDxfId="5"/>
+    <tableColumn id="2" name="rubrique" dataDxfId="4"/>
+    <tableColumn id="3" name="type" dataDxfId="3"/>
+    <tableColumn id="4" name="taille" dataDxfId="2"/>
+    <tableColumn id="5" name="commentaire" dataDxfId="1"/>
+    <tableColumn id="6" name="clé" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1479,369 +1770,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:A59"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7265625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" customWidth="1"/>
-    <col min="22" max="22" width="4.85546875" customWidth="1"/>
-    <col min="23" max="23" width="9" customWidth="1"/>
-    <col min="24" max="25" width="5" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" customWidth="1"/>
-    <col min="27" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8" customWidth="1"/>
-    <col min="31" max="31" width="7.5703125" customWidth="1"/>
-    <col min="32" max="32" width="7" customWidth="1"/>
-    <col min="33" max="33" width="6.85546875" customWidth="1"/>
-    <col min="34" max="34" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.140625" customWidth="1"/>
-    <col min="36" max="36" width="9.85546875" customWidth="1"/>
-    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="16384" width="30.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="30.7109375" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1861,7 +1811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1874,11 +1824,15 @@
       <c r="D3" s="3">
         <v>25</v>
       </c>
+      <c r="E3" s="7" t="str">
+        <f>association!D3</f>
+        <v>Identifiant de l'association</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1891,8 +1845,12 @@
       <c r="D4" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="7" t="str">
+        <f>association!D4</f>
+        <v>Nom de l'association</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1905,8 +1863,12 @@
       <c r="D5" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="7" t="str">
+        <f>association!D5</f>
+        <v>Informations relatives a l'association</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1919,8 +1881,12 @@
       <c r="D6" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="7" t="str">
+        <f>association!D6</f>
+        <v>Adresse e-mail de l'association</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1933,8 +1899,12 @@
       <c r="D7" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="str">
+        <f>association!D7</f>
+        <v>Logo de l'association</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1947,8 +1917,12 @@
       <c r="D8" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="str">
+        <f>association!D8</f>
+        <v>Adresse postale de l'association</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1961,8 +1935,12 @@
       <c r="D9" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="str">
+        <f>association!D9</f>
+        <v>Numéro de téléphone de l'association</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -1975,8 +1953,12 @@
       <c r="D10" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="str">
+        <f>association!D10</f>
+        <v>Adresse du site web de l'association</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1989,8 +1971,12 @@
       <c r="D11" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="str">
+        <f>association!D11</f>
+        <v>Date de création de l'association</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2003,8 +1989,12 @@
       <c r="D12" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="7" t="str">
+        <f>association!D12</f>
+        <v>Numero d'immatriculation de l'association</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -2017,11 +2007,15 @@
       <c r="D13" s="3">
         <v>25</v>
       </c>
+      <c r="E13" s="3" t="str">
+        <f>groupe!D3</f>
+        <v>Identifiant du groupe</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -2034,8 +2028,12 @@
       <c r="D14" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="str">
+        <f>groupe!D4</f>
+        <v>Activité du groupe</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -2048,8 +2046,12 @@
       <c r="D15" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="str">
+        <f>groupe!D5</f>
+        <v>Nom du groupe</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -2062,8 +2064,12 @@
       <c r="D16" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="str">
+        <f>groupe!D6</f>
+        <v>Informations  relatives au groupe</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2076,8 +2082,12 @@
       <c r="D17" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="str">
+        <f>groupe!D7</f>
+        <v>Image associée au groupe</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2090,8 +2100,12 @@
       <c r="D18" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="str">
+        <f>groupe!D8</f>
+        <v>Nombre de membres du groupe</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -2104,8 +2118,12 @@
       <c r="D19" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="str">
+        <f>groupe!D9</f>
+        <v>Type de groupe: interne ou externe</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2118,11 +2136,15 @@
       <c r="D20" s="3">
         <v>11</v>
       </c>
+      <c r="E20" s="3" t="str">
+        <f>groupe!D10</f>
+        <v>Identifiant de l'association</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -2135,11 +2157,15 @@
       <c r="D21" s="3">
         <v>11</v>
       </c>
+      <c r="E21" s="3" t="str">
+        <f>concourrir!D3</f>
+        <v>Identifiant du groupe</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2152,13 +2178,17 @@
       <c r="D22" s="3">
         <v>11</v>
       </c>
+      <c r="E22" s="3" t="str">
+        <f>concourrir!D4</f>
+        <v>Identifiant de la session de jeux</v>
+      </c>
       <c r="F22" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>31</v>
@@ -2169,13 +2199,17 @@
       <c r="D23" s="3">
         <v>25</v>
       </c>
+      <c r="E23" s="3" t="str">
+        <f>session!D3</f>
+        <v>Identifiant de la session de jeu</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>35</v>
@@ -2186,16 +2220,17 @@
       <c r="D24" s="3">
         <v>25</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="3" t="str">
+        <f>session!D4</f>
+        <v>Identifiant du groupe intérieur</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>28</v>
@@ -2203,16 +2238,17 @@
       <c r="D25" s="3">
         <v>25</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="3" t="str">
+        <f>session!D5</f>
+        <v>Identifiant du second groupe (peu être intérieur ou extérieur)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>28</v>
@@ -2220,13 +2256,17 @@
       <c r="D26" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="3" t="str">
+        <f>session!D6</f>
+        <v>Score du groupe A relevé en fin de session</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>28</v>
@@ -2234,13 +2274,17 @@
       <c r="D27" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="str">
+        <f>session!D7</f>
+        <v>Score du groupe B relevé en fin de session</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>19</v>
@@ -2248,16 +2292,20 @@
       <c r="D28" s="3">
         <v>25</v>
       </c>
+      <c r="E28" s="3" t="str">
+        <f>user!D3</f>
+        <v>Identifiant de l'utilisateur</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>20</v>
@@ -2265,13 +2313,17 @@
       <c r="D29" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="3" t="str">
+        <f>user!D4</f>
+        <v>Pseudo de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>20</v>
@@ -2279,13 +2331,17 @@
       <c r="D30" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="3" t="str">
+        <f>user!D5</f>
+        <v>Nom de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>20</v>
@@ -2293,13 +2349,17 @@
       <c r="D31" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="str">
+        <f>user!D6</f>
+        <v>Prénom de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>28</v>
@@ -2307,13 +2367,17 @@
       <c r="D32" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="str">
+        <f>user!D7</f>
+        <v>Numéro de téléphone de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>28</v>
@@ -2321,13 +2385,17 @@
       <c r="D33" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="3" t="str">
+        <f>user!D8</f>
+        <v>Numéro de téléphone portable de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>20</v>
@@ -2335,13 +2403,17 @@
       <c r="D34" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="3" t="str">
+        <f>user!D9</f>
+        <v>Adresse postale de l'uutilisateur</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>20</v>
@@ -2349,13 +2421,17 @@
       <c r="D35" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="3" t="str">
+        <f>user!D10</f>
+        <v>Adresse mail de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>21</v>
@@ -2363,13 +2439,17 @@
       <c r="D36" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="3" t="str">
+        <f>user!D11</f>
+        <v>Date de naissance de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>28</v>
@@ -2377,13 +2457,17 @@
       <c r="D37" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="str">
+        <f>user!D12</f>
+        <v>Type de compte: Licencié, non licencié, administrateur, gestionnaire…</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>20</v>
@@ -2391,13 +2475,17 @@
       <c r="D38" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="3" t="str">
+        <f>user!D13</f>
+        <v>Mot de passe de l'utilisateur</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>28</v>
@@ -2405,13 +2493,17 @@
       <c r="D39" s="3">
         <v>11</v>
       </c>
+      <c r="E39" s="3" t="str">
+        <f>user!D14</f>
+        <v>Identifiant de la license utilisateur</v>
+      </c>
       <c r="F39" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>18</v>
@@ -2422,16 +2514,20 @@
       <c r="D40" s="3">
         <v>11</v>
       </c>
+      <c r="E40" s="3" t="str">
+        <f>user!D15</f>
+        <v>Identifiant du groupe de l'utilisateur</v>
+      </c>
       <c r="F40" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>19</v>
@@ -2439,16 +2535,20 @@
       <c r="D41" s="3">
         <v>25</v>
       </c>
+      <c r="E41" s="3" t="str">
+        <f>license!D3</f>
+        <v>Identifiant de licence</v>
+      </c>
       <c r="F41" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>20</v>
@@ -2456,13 +2556,17 @@
       <c r="D42" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="3" t="str">
+        <f>license!D4</f>
+        <v>Type de licence (0, 1, 2) pour le renouvellement des licence  (e-mail)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>21</v>
@@ -2470,13 +2574,17 @@
       <c r="D43" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="3" t="str">
+        <f>license!D5</f>
+        <v>Date d'acquisition de la licence</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>28</v>
@@ -2484,16 +2592,20 @@
       <c r="D44" s="3">
         <v>11</v>
       </c>
+      <c r="E44" s="3" t="str">
+        <f>license!D6</f>
+        <v>Identifiant de l'utilisateur</v>
+      </c>
       <c r="F44" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>28</v>
@@ -2501,16 +2613,20 @@
       <c r="D45" s="3">
         <v>11</v>
       </c>
+      <c r="E45" s="3" t="str">
+        <f>license!D7</f>
+        <v>Identifiant du paiement de la licence</v>
+      </c>
       <c r="F45" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>19</v>
@@ -2518,16 +2634,20 @@
       <c r="D46" s="3">
         <v>25</v>
       </c>
+      <c r="E46" s="3" t="str">
+        <f>paiement!D3</f>
+        <v>Identifiant de la licence</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>28</v>
@@ -2535,27 +2655,35 @@
       <c r="D47" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="3" t="str">
+        <f>paiement!D4</f>
+        <v>Type de règlement (espece, CB, chéque)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D48" s="3">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="3" t="str">
+        <f>paiement!D5</f>
+        <v>Montant du paiement</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>21</v>
@@ -2563,19 +2691,27 @@
       <c r="D49" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="3" t="str">
+        <f>paiement!D6</f>
+        <v>Date du paiment</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D50" s="3">
         <v>11</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f>paiement!D7</f>
+        <v>Identifiant de licence</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>34</v>
@@ -2591,4 +2727,1423 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" customWidth="1"/>
+    <col min="4" max="5" width="8.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.81640625" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="9.26953125" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" customWidth="1"/>
+    <col min="17" max="17" width="6.54296875" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" customWidth="1"/>
+    <col min="19" max="19" width="6.81640625" customWidth="1"/>
+    <col min="20" max="20" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" customWidth="1"/>
+    <col min="22" max="22" width="4.81640625" customWidth="1"/>
+    <col min="23" max="23" width="9" customWidth="1"/>
+    <col min="24" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="9.1796875" customWidth="1"/>
+    <col min="27" max="28" width="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8" customWidth="1"/>
+    <col min="31" max="31" width="7.54296875" customWidth="1"/>
+    <col min="32" max="32" width="7" customWidth="1"/>
+    <col min="33" max="33" width="6.81640625" customWidth="1"/>
+    <col min="34" max="34" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.1796875" customWidth="1"/>
+    <col min="36" max="36" width="9.81640625" customWidth="1"/>
+    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7">
+        <v>100</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7">
+        <v>100</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7">
+        <v>60</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7">
+        <v>200</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>50</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7">
+        <v>60</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7">
+        <v>100</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7">
+        <v>100</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7">
+        <v>25</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="7">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7">
+        <v>50</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="7">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="7">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="21.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="7">
+        <v>25.2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>